<commit_message>
It is fully build. Most Errors are handled and missing ones will be further handled
</commit_message>
<xml_diff>
--- a/Report Creator/test_subjects/Marks Sheet Term II 2024/O level Marks Sheet Term II 2024/Marksheet O level - PHYSICS.xlsx
+++ b/Report Creator/test_subjects/Marks Sheet Term II 2024/O level Marks Sheet Term II 2024/Marksheet O level - PHYSICS.xlsx
@@ -486,10 +486,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -764,7 +764,9 @@
         <v>8</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="2">
+        <v>20.0</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="G3" s="1"/>
     </row>
@@ -773,7 +775,9 @@
         <v>9</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2">
+        <v>60.0</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
     </row>
@@ -782,7 +786,9 @@
         <v>10</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2">
+        <v>20.0</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
     </row>
@@ -791,7 +797,9 @@
         <v>11</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2">
+        <v>80.0</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
     </row>
@@ -800,7 +808,9 @@
         <v>12</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2">
+        <v>80.0</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="G7" s="1"/>
     </row>
@@ -809,7 +819,9 @@
         <v>13</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2">
+        <v>50.0</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="G8" s="1"/>
     </row>
@@ -818,7 +830,9 @@
         <v>14</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2">
+        <v>80.0</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="G9" s="1"/>
     </row>
@@ -836,7 +850,9 @@
         <v>16</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2">
+        <v>40.0</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="G11" s="1"/>
     </row>
@@ -845,7 +861,9 @@
         <v>17</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2">
+        <v>50.0</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="G12" s="1"/>
     </row>
@@ -854,7 +872,9 @@
         <v>18</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2">
+        <v>20.0</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="G13" s="1"/>
     </row>
@@ -863,7 +883,9 @@
         <v>19</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2">
+        <v>30.0</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="G14" s="1"/>
     </row>
@@ -881,7 +903,9 @@
         <v>21</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2">
+        <v>60.0</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="G16" s="1"/>
     </row>
@@ -890,7 +914,9 @@
         <v>22</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="2">
+        <v>20.0</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="G17" s="1"/>
     </row>
@@ -899,7 +925,9 @@
         <v>23</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="2">
+        <v>50.0</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19">
@@ -934,7 +962,9 @@
         <v>27</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="2">
+        <v>30.0</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="G22" s="1"/>
     </row>
@@ -952,7 +982,9 @@
         <v>29</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="2">
+        <v>30.0</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="G24" s="1"/>
     </row>
@@ -961,7 +993,9 @@
         <v>30</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="D25" s="2">
+        <v>80.0</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="G25" s="1"/>
     </row>
@@ -979,7 +1013,9 @@
         <v>32</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="D27" s="2">
+        <v>65.0</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="G27" s="1"/>
     </row>
@@ -988,7 +1024,9 @@
         <v>33</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="D28" s="2">
+        <v>50.0</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="G28" s="1"/>
     </row>
@@ -1015,12 +1053,14 @@
         <v>36</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="D31" s="2">
+        <v>60.0</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2436,7 +2476,7 @@
       <c r="F51" s="1"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3413,7 +3453,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3440,7 +3480,9 @@
         <v>88</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="D2" s="2">
+        <v>40.0</v>
+      </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3">
@@ -3448,7 +3490,9 @@
         <v>89</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="2">
+        <v>80.0</v>
+      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4">
@@ -3456,7 +3500,9 @@
         <v>90</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2">
+        <v>30.0</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
@@ -3464,7 +3510,9 @@
         <v>91</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2">
+        <v>40.0</v>
+      </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6">
@@ -3472,7 +3520,9 @@
         <v>92</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2">
+        <v>70.0</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7">
@@ -3480,7 +3530,9 @@
         <v>93</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2">
+        <v>40.0</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8">
@@ -3488,7 +3540,9 @@
         <v>94</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2">
+        <v>30.0</v>
+      </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9">
@@ -3496,7 +3550,9 @@
         <v>95</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2">
+        <v>30.0</v>
+      </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10">
@@ -3520,7 +3576,9 @@
         <v>98</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2">
+        <v>70.0</v>
+      </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
@@ -3528,7 +3586,9 @@
         <v>99</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2">
+        <v>30.0</v>
+      </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14">
@@ -3536,7 +3596,9 @@
         <v>100</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2">
+        <v>40.0</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15">
@@ -3544,7 +3606,9 @@
         <v>101</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2">
+        <v>30.0</v>
+      </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16">
@@ -3552,7 +3616,9 @@
         <v>102</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2">
+        <v>40.0</v>
+      </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17">
@@ -3560,7 +3626,9 @@
         <v>103</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="2">
+        <v>30.0</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18">
@@ -3568,14 +3636,18 @@
         <v>104</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="2">
+        <v>40.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="2">
+        <v>40.0</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20">
@@ -3583,7 +3655,9 @@
         <v>106</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="2">
+        <v>80.0</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -3591,7 +3665,9 @@
         <v>107</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="2">
+        <v>30.0</v>
+      </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -3599,7 +3675,9 @@
         <v>108</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="2">
+        <v>30.0</v>
+      </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -3615,7 +3693,9 @@
         <v>110</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="2">
+        <v>70.0</v>
+      </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -3630,7 +3710,9 @@
         <v>112</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="D26" s="2">
+        <v>80.0</v>
+      </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -3638,7 +3720,9 @@
         <v>113</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="D27" s="2">
+        <v>30.0</v>
+      </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -3646,7 +3730,9 @@
         <v>114</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="D28" s="2">
+        <v>80.0</v>
+      </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -3654,7 +3740,9 @@
         <v>115</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="D29" s="2">
+        <v>40.0</v>
+      </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -3670,7 +3758,9 @@
         <v>117</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="D31" s="2">
+        <v>40.0</v>
+      </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -3678,7 +3768,9 @@
         <v>118</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="D32" s="2">
+        <v>70.0</v>
+      </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -3686,7 +3778,9 @@
         <v>119</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="D33" s="2">
+        <v>70.0</v>
+      </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -3694,7 +3788,9 @@
         <v>120</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="D34" s="2">
+        <v>40.0</v>
+      </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -3702,11 +3798,13 @@
         <v>121</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="D35" s="2">
+        <v>80.0</v>
+      </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4699,7 +4797,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -4896,7 +4994,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>